<commit_message>
reflector the cucumber test
</commit_message>
<xml_diff>
--- a/src/app/app-pl/test/TestCase.xlsx
+++ b/src/app/app-pl/test/TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/njs/njstool/src/app/app-pl/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FC0974-03CA-E44A-9C7A-5F39DF44FFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C13C815-DCAC-1440-8D2D-422BB729CECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="17500" xr2:uid="{5EC04115-4F26-5F43-A035-0399DF9533CE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>type</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>settled</t>
+  </si>
+  <si>
+    <t>book price</t>
   </si>
 </sst>
 </file>
@@ -451,25 +454,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B4DCDE-4CB1-C44F-BA69-12FC166E2826}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="6" max="6" width="5.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -489,22 +493,25 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45658</v>
       </c>
@@ -525,7 +532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45662</v>
       </c>
@@ -537,25 +544,29 @@
         <v>100</v>
       </c>
       <c r="H4">
+        <f>D3</f>
+        <v>10</v>
+      </c>
+      <c r="I4">
         <f>SUM(E3:E4)</f>
         <v>1000</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>13</v>
       </c>
-      <c r="J4">
-        <f>G4*I4</f>
+      <c r="K4">
+        <f>G4*J4</f>
         <v>1300</v>
       </c>
-      <c r="K4">
-        <f>J4-H4</f>
+      <c r="L4">
+        <f>K4-I4</f>
         <v>300</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45689</v>
       </c>
@@ -575,26 +586,26 @@
       <c r="G5">
         <v>100</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f>SUM(E3:E4)</f>
         <v>1000</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>12</v>
       </c>
-      <c r="J5">
-        <f>I5*G5</f>
+      <c r="K5">
+        <f>J5*G5</f>
         <v>1200</v>
       </c>
-      <c r="K5">
-        <f>J5-H5</f>
+      <c r="L5">
+        <f>K5-I5</f>
         <v>200</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>45693</v>
       </c>
@@ -604,26 +615,26 @@
       <c r="G6">
         <v>150</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f>SUM(E3:E5)</f>
         <v>1650</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>14</v>
       </c>
-      <c r="J6">
-        <f>I6*G6</f>
+      <c r="K6">
+        <f>J6*G6</f>
         <v>2100</v>
       </c>
-      <c r="K6">
-        <f>J6-H6</f>
+      <c r="L6">
+        <f>K6-I6</f>
         <v>450</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45717</v>
       </c>
@@ -643,26 +654,26 @@
       <c r="G7">
         <v>150</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f>SUM(E3:E6)</f>
         <v>1650</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>14</v>
       </c>
-      <c r="J7">
-        <f>I7*G7</f>
+      <c r="K7">
+        <f>J7*G7</f>
         <v>2100</v>
       </c>
-      <c r="K7">
-        <f>J7-H7</f>
+      <c r="L7">
+        <f>K7-I7</f>
         <v>450</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45721</v>
       </c>
@@ -673,27 +684,27 @@
         <f>SUM(C3:C8)</f>
         <v>70</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f>SUM(E3:E7)</f>
         <v>850</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>17</v>
       </c>
-      <c r="J8">
-        <f>I8*G8</f>
+      <c r="K8">
+        <f>J8*G8</f>
         <v>1190</v>
       </c>
-      <c r="K8">
-        <f>J8-H8</f>
+      <c r="L8">
+        <f>K8-I8</f>
         <v>340</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f>(D7-D3)*(C3+C7)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>45748</v>
       </c>
@@ -714,27 +725,27 @@
         <f>G8</f>
         <v>70</v>
       </c>
-      <c r="H9">
-        <f>H8</f>
+      <c r="I9">
+        <f>I8</f>
         <v>850</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>16</v>
       </c>
-      <c r="J9">
-        <f>I9*G9</f>
+      <c r="K9">
+        <f>J9*G9</f>
         <v>1120</v>
       </c>
-      <c r="K9">
-        <f>J9-H9</f>
+      <c r="L9">
+        <f>K9-I9</f>
         <v>270</v>
       </c>
-      <c r="L9">
-        <f>L8</f>
+      <c r="M9">
+        <f>M8</f>
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45752</v>
       </c>
@@ -745,27 +756,27 @@
         <f>SUM(C3:C9)</f>
         <v>120</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <f>SUM(E3:E9)</f>
         <v>1650</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>13</v>
       </c>
-      <c r="J10">
-        <f>I10*G10</f>
+      <c r="K10">
+        <f>J10*G10</f>
         <v>1560</v>
       </c>
-      <c r="K10">
-        <f>J10-H10</f>
+      <c r="L10">
+        <f>K10-I10</f>
         <v>-90</v>
       </c>
-      <c r="L10">
-        <f>L9</f>
+      <c r="M10">
+        <f>M9</f>
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>45778</v>
       </c>
@@ -786,27 +797,27 @@
         <f>G10</f>
         <v>120</v>
       </c>
-      <c r="H11">
-        <f>H10</f>
+      <c r="I11">
+        <f>I10</f>
         <v>1650</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>11</v>
       </c>
-      <c r="J11">
-        <f>I11*G11</f>
+      <c r="K11">
+        <f>J11*G11</f>
         <v>1320</v>
       </c>
-      <c r="K11">
-        <f>J11-H11</f>
+      <c r="L11">
+        <f>K11-I11</f>
         <v>-330</v>
       </c>
-      <c r="L11">
-        <f>L10</f>
+      <c r="M11">
+        <f>M10</f>
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45782</v>
       </c>
@@ -817,22 +828,22 @@
         <f>SUM(C3:C11)</f>
         <v>80</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f>SUM(E3:E11)</f>
         <v>1190</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>9</v>
       </c>
-      <c r="J12">
-        <f>I12*G12</f>
+      <c r="K12">
+        <f>J12*G12</f>
         <v>720</v>
       </c>
-      <c r="K12">
-        <f>J12-H12</f>
+      <c r="L12">
+        <f>K12-I12</f>
         <v>-470</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <f>(D11*C11*-1)+E11</f>
         <v>-20</v>
       </c>

</xml_diff>